<commit_message>
implementation of withdraw apply
</commit_message>
<xml_diff>
--- a/web/material/template/withdraw_apply_template.xlsx
+++ b/web/material/template/withdraw_apply_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>提现申请</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t>申请时间</t>
+  </si>
+  <si>
+    <t>提款渠道</t>
+  </si>
+  <si>
+    <t>提款账号</t>
+  </si>
+  <si>
+    <t>下载时间</t>
   </si>
 </sst>
 </file>
@@ -65,7 +74,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -88,16 +97,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -377,49 +436,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implementation of withdraw apply record download
</commit_message>
<xml_diff>
--- a/web/material/template/withdraw_apply_template.xlsx
+++ b/web/material/template/withdraw_apply_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -138,14 +138,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -153,10 +158,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -439,32 +440,37 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="6" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -479,10 +485,10 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>